<commit_message>
chore: update metrics files
</commit_message>
<xml_diff>
--- a/Evaluate_TTACT/PR_Comparison.xlsx
+++ b/Evaluate_TTACT/PR_Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Stuff\VIT-20BCE1789\Sem 8\Capstone\Work\frontend\Evaluate_TTACT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232894B7-E086-47C2-8A73-B409DA023D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A93F0B-EB7B-4218-8277-6F76EDB35C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,13 +34,7 @@
     <t>TTACT</t>
   </si>
   <si>
-    <t>NISA</t>
-  </si>
-  <si>
     <t>AUC</t>
-  </si>
-  <si>
-    <t>WM + ML</t>
   </si>
   <si>
     <t>TTACT - new v1</t>
@@ -68,6 +62,12 @@
   </si>
   <si>
     <t>TTACT New v9</t>
+  </si>
+  <si>
+    <t>WM + ML [16]</t>
+  </si>
+  <si>
+    <t>NISA [17]</t>
   </si>
 </sst>
 </file>
@@ -873,7 +873,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>WM + ML</c:v>
+                  <c:v>WM + ML [16]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1050,7 +1050,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NISA</c:v>
+                  <c:v>NISA [17]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2466,8 +2466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M149" sqref="M149"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25">
         <v>0.96245245287507197</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -2981,7 +2981,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B52">
         <v>0.96536758153020397</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -3236,7 +3236,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B78">
         <v>0.803877603492969</v>
@@ -3244,7 +3244,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -3491,7 +3491,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B105">
         <v>0.96111047426232399</v>
@@ -3499,16 +3499,16 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
+        <v>6</v>
+      </c>
+      <c r="F108" t="s">
+        <v>7</v>
+      </c>
+      <c r="K108" t="s">
         <v>8</v>
       </c>
-      <c r="F108" t="s">
+      <c r="P108" t="s">
         <v>9</v>
-      </c>
-      <c r="K108" t="s">
-        <v>10</v>
-      </c>
-      <c r="P108" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.3">
@@ -4349,25 +4349,25 @@
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B132">
         <v>0.96111047426232399</v>
       </c>
       <c r="F132" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G132">
         <v>0.96111047426232399</v>
       </c>
       <c r="K132" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L132">
         <v>0.95626836919375502</v>
       </c>
       <c r="P132" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q132">
         <v>0.94913012702467703</v>
@@ -4375,16 +4375,16 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
+        <v>10</v>
+      </c>
+      <c r="F137" t="s">
+        <v>11</v>
+      </c>
+      <c r="K137" t="s">
         <v>12</v>
       </c>
-      <c r="F137" t="s">
+      <c r="P137" t="s">
         <v>13</v>
-      </c>
-      <c r="K137" t="s">
-        <v>14</v>
-      </c>
-      <c r="P137" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.3">
@@ -5225,25 +5225,25 @@
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B161">
         <v>0.94387695400105498</v>
       </c>
       <c r="F161" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G161">
         <v>0.96468272505907704</v>
       </c>
       <c r="K161" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L161">
         <v>0.96468272505907704</v>
       </c>
       <c r="P161" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q161">
         <v>0.96468272505907704</v>

</xml_diff>